<commit_message>
Update metadata of stimmbeteiligung dataset
</commit_message>
<xml_diff>
--- a/automation/stimmbeteiligung/Meta_Stimmbeteiligung.xlsx
+++ b/automation/stimmbeteiligung/Meta_Stimmbeteiligung.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16623" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16626" uniqueCount="159">
   <si>
     <t>Erstmalige Veröffentlichung</t>
   </si>
@@ -631,6 +631,16 @@
 </t>
     </r>
   </si>
+  <si>
+    <t>Die Stimmbeteiligung vor einem Urnengang wird anhand der eingegangenen brieflichen Abstimmungsunterlagen bestimmt Die Stadtkanzlei misst dabei die Höhe der eingegangenen Couverts und schätzt die Anzahl Couverts. Die Prozentwerte sind somit nicht nicht sehr genau und mit Vorsicht zu verwenden.</t>
+  </si>
+  <si>
+    <t>Genauigkeit der Werte</t>
+  </si>
+  <si>
+    <t>Die Stimmbeteiligung wird von der Stadtkanzlei anhand der Höhe der eingegangen brieflichen Abstimmungsunterlagen geschätzt. Diese Methode ist sehr einfach und gibt Aufschluss über den generallen Trend der Stimmbeteiligung.
+Weil es sich dabei aber um Schätzungen handelt, sind die Werte mit Vorsicht zu verwenden.</t>
+  </si>
 </sst>
 </file>
 
@@ -1235,10 +1245,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:XFD44"/>
+  <dimension ref="A1:XFD45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="255.5" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1412,7 +1422,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" s="4" customFormat="1" ht="50" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
         <v>39</v>
       </c>
@@ -1420,7 +1430,9 @@
         <v>15</v>
       </c>
       <c r="C10" s="21"/>
-      <c r="D10" s="22"/>
+      <c r="D10" s="22" t="s">
+        <v>156</v>
+      </c>
       <c r="E10" s="9" t="s">
         <v>57</v>
       </c>
@@ -50730,127 +50742,128 @@
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="1:16384" ht="78" x14ac:dyDescent="0.3">
-      <c r="A22" s="13" t="s">
+    <row r="22" spans="1:16384" ht="91" x14ac:dyDescent="0.3">
+      <c r="B22" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="C22" s="26" t="s">
+        <v>158</v>
+      </c>
+      <c r="D22" s="26"/>
+      <c r="E22" s="28"/>
+    </row>
+    <row r="23" spans="1:16384" ht="78" x14ac:dyDescent="0.3">
+      <c r="A23" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="B22" s="26" t="s">
+      <c r="B23" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="C22" s="26" t="s">
+      <c r="C23" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="D22" s="26"/>
+      <c r="D23" s="26"/>
     </row>
-    <row r="23" spans="1:16384" x14ac:dyDescent="0.3">
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-    </row>
-    <row r="24" spans="1:16384" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A24" s="13"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="8"/>
+    <row r="24" spans="1:16384" x14ac:dyDescent="0.3">
+      <c r="B24" s="16"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
     </row>
     <row r="25" spans="1:16384" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A25" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10" t="s">
-        <v>22</v>
-      </c>
+      <c r="A25" s="13"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="8"/>
     </row>
     <row r="26" spans="1:16384" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A26" s="13"/>
-      <c r="B26" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C26" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D26" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>33</v>
+      <c r="A26" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:16384" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A27" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B27" s="26" t="s">
-        <v>146</v>
-      </c>
-      <c r="C27" s="26" t="s">
-        <v>152</v>
-      </c>
-      <c r="D27" s="26" t="s">
-        <v>147</v>
+      <c r="A27" s="13"/>
+      <c r="B27" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>84</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:16384" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16384" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A28" s="13" t="s">
         <v>35</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C28" s="26" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D28" s="26" t="s">
-        <v>150</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>86</v>
+        <v>147</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:16384" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16384" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A29" s="13" t="s">
         <v>35</v>
       </c>
       <c r="B29" s="26" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C29" s="26" t="s">
-        <v>4</v>
+        <v>149</v>
       </c>
       <c r="D29" s="26" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:16384" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A30" s="13"/>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
+      <c r="A30" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="C30" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>85</v>
+      </c>
       <c r="F30" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:16384" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
@@ -50858,6 +50871,9 @@
       <c r="B31" s="26"/>
       <c r="C31" s="26"/>
       <c r="D31" s="26"/>
+      <c r="F31" s="4" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="32" spans="1:16384" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A32" s="13"/>
@@ -50889,11 +50905,11 @@
       <c r="C36" s="26"/>
       <c r="D36" s="26"/>
     </row>
-    <row r="37" spans="1:4" s="4" customFormat="1" ht="12.5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A37" s="13"/>
-      <c r="B37" s="15"/>
-      <c r="C37" s="15"/>
-      <c r="D37" s="15"/>
+      <c r="B37" s="26"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="26"/>
     </row>
     <row r="38" spans="1:4" s="4" customFormat="1" ht="12.5" x14ac:dyDescent="0.3">
       <c r="A38" s="13"/>
@@ -50913,11 +50929,11 @@
       <c r="C40" s="15"/>
       <c r="D40" s="15"/>
     </row>
-    <row r="41" spans="1:4" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" s="4" customFormat="1" ht="12.5" x14ac:dyDescent="0.3">
       <c r="A41" s="13"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="8"/>
+      <c r="B41" s="15"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15"/>
     </row>
     <row r="42" spans="1:4" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A42" s="13"/>
@@ -50935,7 +50951,13 @@
       <c r="A44" s="13"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
-      <c r="D44" s="7"/>
+      <c r="D44" s="8"/>
+    </row>
+    <row r="45" spans="1:4" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+      <c r="A45" s="13"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.98425196850393704" bottom="0.59055118110236227" header="0.39370078740157483" footer="0.27559055118110237"/>
@@ -51512,12 +51534,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -51635,15 +51654,25 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4B3AD83-9986-4E71-995F-A94C1CED6EB8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6056489-A7A4-4445-AFC5-87E5586E5E93}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -51665,16 +51694,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6056489-A7A4-4445-AFC5-87E5586E5E93}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4B3AD83-9986-4E71-995F-A94C1CED6EB8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update Link to Abstimmungsresultate
</commit_message>
<xml_diff>
--- a/automation/stimmbeteiligung/Meta_Stimmbeteiligung.xlsx
+++ b/automation/stimmbeteiligung/Meta_Stimmbeteiligung.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\dev\opendatazurich.github.io\automation\stimmbeteiligung\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sszgua\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AE25B1B-032A-4765-905E-156EB0D832A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="-45" windowWidth="21225" windowHeight="12540"/>
+    <workbookView xWindow="1065" yWindow="-120" windowWidth="27855" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="14" r:id="rId1"/>
@@ -579,9 +580,6 @@
     <t>14.06.2021</t>
   </si>
   <si>
-    <t>Die Stimmbeteiligung wird vor einem Urnengang regelmässig aktualisiert. Die tatsächlichen Abstimmungsergebnisse und die Stimmbeteiligung werden nach dem Abstimmungstermin im Datensatz ["Abstimmungsresultate seit 1933"](/dataset/politik-abstimmungen-seit-1933) zur Verfügung gestellt.</t>
-  </si>
-  <si>
     <t>Abstimmungs_Datum</t>
   </si>
   <si>
@@ -637,11 +635,14 @@
   <si>
     <t>Dieser Wert beruht auf der aktuellen Zahl der durch die Post verarbeiteten und der in den Briefkasten des Stadthauses eingelegten Antwortkuverts. Die effektive Stimm-/Wahlbeteiligung inkl. persönlicher Stimmabgabe an der Urne steht erst nach der Auszählung am Abstimmungssonntag fest.</t>
   </si>
+  <si>
+    <t>Die Stimmbeteiligung wird vor einem Urnengang regelmässig aktualisiert. Die tatsächlichen Abstimmungsergebnisse und die Stimmbeteiligung werden nach dem Abstimmungstermin im Datensatz ["Abstimmungsresultate seit 1933"](/dataset/politik_abstimmungen_seit1933) zur Verfügung gestellt.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -996,10 +997,10 @@
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Standard 2" xfId="1"/>
-    <cellStyle name="Standard 3" xfId="2"/>
-    <cellStyle name="Standard 4" xfId="3"/>
-    <cellStyle name="Standard 5" xfId="4"/>
+    <cellStyle name="Standard 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Standard 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Standard 4" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Standard 5" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1240,11 +1241,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:XFD45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="255.5" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1305,7 +1306,7 @@
       </c>
       <c r="C3" s="20"/>
       <c r="D3" s="27" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>73</v>
@@ -1427,7 +1428,7 @@
       </c>
       <c r="C10" s="21"/>
       <c r="D10" s="22" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>57</v>
@@ -1555,7 +1556,7 @@
         <v>19</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>135</v>
@@ -50743,15 +50744,15 @@
         <v>68</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C22" s="26" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D22" s="26"/>
       <c r="E22" s="28"/>
     </row>
-    <row r="23" spans="1:16384" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16384" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A23" s="13" t="s">
         <v>68</v>
       </c>
@@ -50759,7 +50760,7 @@
         <v>139</v>
       </c>
       <c r="C23" s="26" t="s">
-        <v>145</v>
+        <v>157</v>
       </c>
       <c r="D23" s="26"/>
     </row>
@@ -50813,13 +50814,13 @@
         <v>35</v>
       </c>
       <c r="B28" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="C28" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="D28" s="26" t="s">
         <v>146</v>
-      </c>
-      <c r="C28" s="26" t="s">
-        <v>151</v>
-      </c>
-      <c r="D28" s="26" t="s">
-        <v>147</v>
       </c>
       <c r="F28" s="4" t="s">
         <v>52</v>
@@ -50830,13 +50831,13 @@
         <v>35</v>
       </c>
       <c r="B29" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="C29" s="26" t="s">
         <v>148</v>
       </c>
-      <c r="C29" s="26" t="s">
-        <v>149</v>
-      </c>
       <c r="D29" s="26" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>86</v>
@@ -50850,13 +50851,13 @@
         <v>35</v>
       </c>
       <c r="B30" s="26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C30" s="26" t="s">
         <v>4</v>
       </c>
       <c r="D30" s="26" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>85</v>
@@ -50965,7 +50966,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
@@ -51542,6 +51543,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101008CBAF0EEED2F5B4AB4463B97C2AD2B71" ma:contentTypeVersion="0" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="d2bc9691d179cb44d4ba77bdf8fcfb4a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="66c4a6dd5ef775a5269b08f7de37f93f">
     <xsd:element name="properties">
@@ -51655,12 +51662,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4B3AD83-9986-4E71-995F-A94C1CED6EB8}">
   <ds:schemaRefs>
@@ -51670,6 +51671,21 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6056489-A7A4-4445-AFC5-87E5586E5E93}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F33FC2A8-E9AF-48AF-8CDC-2C0CCE48C45D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -51683,19 +51699,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6056489-A7A4-4445-AFC5-87E5586E5E93}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>